<commit_message>
Copied cleaned up code everywhere
</commit_message>
<xml_diff>
--- a/Code/SampleRun_Environment_Wind/100Scens/100_Naive_CI.xlsx
+++ b/Code/SampleRun_Environment_Wind/100Scens/100_Naive_CI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Dokumente\A_Uni\HiWi\ArticleSubgradient\Code\SampleRun_Environment_Wind\100Scens\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01AB5FCC-9023-44AF-8CE8-9E23262473B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FA0568-E836-4A08-B255-A4F0F009FB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -442,7 +442,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F121"/>
   <sheetViews>
     <sheetView topLeftCell="A106" workbookViewId="0">
@@ -2584,11 +2584,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:Q8"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2613,7 +2613,7 @@
         <v>5</v>
       </c>
       <c r="L1" s="1">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.35">

</xml_diff>